<commit_message>
Menambahkan file latihan chapter 3 dan 4
</commit_message>
<xml_diff>
--- a/Latihan Chapter 2.xlsx
+++ b/Latihan Chapter 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Excel Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FAC2B7-29E0-45F8-9B5D-83EFE1AC39A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F8F80B-1FA5-44D9-877F-40F1BBE9025E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{60108C04-1B18-43F2-A49F-44C6908738B1}"/>
+    <workbookView xWindow="345" yWindow="780" windowWidth="28455" windowHeight="10635" xr2:uid="{60108C04-1B18-43F2-A49F-44C6908738B1}"/>
   </bookViews>
   <sheets>
     <sheet name="daftar_hadir" sheetId="1" r:id="rId1"/>
@@ -427,12 +427,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -451,6 +445,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -769,7 +769,7 @@
   <dimension ref="B2:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="B2" sqref="B2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,19 +782,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="12"/>
       <c r="E4" t="s">
         <v>5</v>
       </c>
@@ -813,318 +813,318 @@
       </c>
     </row>
     <row r="8" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="8">
+      <c r="B9" s="6">
         <v>1</v>
       </c>
-      <c r="C9" s="6" t="str">
+      <c r="C9" s="4" t="str">
         <f>PROPER(daftar_member!B4)</f>
         <v>Arya Putra</v>
       </c>
-      <c r="D9" s="8" t="str">
+      <c r="D9" s="6" t="str">
         <f>UPPER(LEFT(C9,2))</f>
         <v>AR</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="7">
         <v>38263</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="8" t="s">
         <v>8</v>
       </c>
       <c r="J9" s="3"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="8">
+      <c r="B10" s="6">
         <v>2</v>
       </c>
-      <c r="C10" s="6" t="str">
+      <c r="C10" s="4" t="str">
         <f>PROPER(daftar_member!B5)</f>
         <v>Nadia Rahma</v>
       </c>
-      <c r="D10" s="8" t="str">
+      <c r="D10" s="6" t="str">
         <f t="shared" ref="D10:D23" si="0">UPPER(LEFT(C10,2))</f>
         <v>NA</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="8" t="s">
         <v>9</v>
       </c>
       <c r="J10" s="3"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="8">
+      <c r="B11" s="6">
         <v>3</v>
       </c>
-      <c r="C11" s="6" t="str">
+      <c r="C11" s="4" t="str">
         <f>PROPER(daftar_member!B6)</f>
         <v>Budi Santoso</v>
       </c>
-      <c r="D11" s="8" t="str">
+      <c r="D11" s="6" t="str">
         <f t="shared" si="0"/>
         <v>BU</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="7">
         <v>38474</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="8" t="s">
         <v>10</v>
       </c>
       <c r="J11" s="3"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="8">
+      <c r="B12" s="6">
         <v>4</v>
       </c>
-      <c r="C12" s="6" t="str">
+      <c r="C12" s="4" t="str">
         <f>PROPER(daftar_member!B7)</f>
         <v>Siti Aminah</v>
       </c>
-      <c r="D12" s="8" t="str">
+      <c r="D12" s="6" t="str">
         <f t="shared" si="0"/>
         <v>SI</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="7">
         <v>37474</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="8" t="s">
         <v>11</v>
       </c>
       <c r="J12" s="3"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="8">
+      <c r="B13" s="6">
         <v>5</v>
       </c>
-      <c r="C13" s="6" t="str">
+      <c r="C13" s="4" t="str">
         <f>PROPER(daftar_member!B8)</f>
         <v>Riko Pratama</v>
       </c>
-      <c r="D13" s="8" t="str">
+      <c r="D13" s="6" t="str">
         <f t="shared" si="0"/>
         <v>RI</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="8" t="s">
         <v>12</v>
       </c>
       <c r="J13" s="3"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="8">
+      <c r="B14" s="6">
         <v>6</v>
       </c>
-      <c r="C14" s="6" t="str">
+      <c r="C14" s="4" t="str">
         <f>PROPER(daftar_member!B9)</f>
         <v>Lina Kusuma</v>
       </c>
-      <c r="D14" s="8" t="str">
+      <c r="D14" s="6" t="str">
         <f t="shared" si="0"/>
         <v>LI</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="7">
         <v>37960</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="8" t="s">
         <v>13</v>
       </c>
       <c r="J14" s="3"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="8">
+      <c r="B15" s="6">
         <v>7</v>
       </c>
-      <c r="C15" s="6" t="str">
+      <c r="C15" s="4" t="str">
         <f>PROPER(daftar_member!B10)</f>
         <v>Fajar Hidayat</v>
       </c>
-      <c r="D15" s="8" t="str">
+      <c r="D15" s="6" t="str">
         <f t="shared" si="0"/>
         <v>FA</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="8" t="s">
         <v>14</v>
       </c>
       <c r="J15" s="3"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="8">
+      <c r="B16" s="6">
         <v>8</v>
       </c>
-      <c r="C16" s="6" t="str">
+      <c r="C16" s="4" t="str">
         <f>PROPER(daftar_member!B11)</f>
         <v>Maya Sari</v>
       </c>
-      <c r="D16" s="8" t="str">
+      <c r="D16" s="6" t="str">
         <f t="shared" si="0"/>
         <v>MA</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="8" t="s">
         <v>15</v>
       </c>
       <c r="J16" s="3"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="8">
+      <c r="B17" s="6">
         <v>9</v>
       </c>
-      <c r="C17" s="6" t="str">
+      <c r="C17" s="4" t="str">
         <f>PROPER(daftar_member!B12)</f>
         <v>Agus Kurniawan</v>
       </c>
-      <c r="D17" s="8" t="str">
+      <c r="D17" s="6" t="str">
         <f t="shared" si="0"/>
         <v>AG</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="8" t="s">
         <v>16</v>
       </c>
       <c r="J17" s="3"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="8">
+      <c r="B18" s="6">
         <v>10</v>
       </c>
-      <c r="C18" s="6" t="str">
+      <c r="C18" s="4" t="str">
         <f>PROPER(daftar_member!B13)</f>
         <v>Fitri Nursanti</v>
       </c>
-      <c r="D18" s="8" t="str">
+      <c r="D18" s="6" t="str">
         <f t="shared" si="0"/>
         <v>FI</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="7">
         <v>38272</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="8" t="s">
         <v>17</v>
       </c>
       <c r="J18" s="3"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="8">
+      <c r="B19" s="6">
         <v>11</v>
       </c>
-      <c r="C19" s="6" t="str">
+      <c r="C19" s="4" t="str">
         <f>PROPER(daftar_member!B14)</f>
         <v>Dimas Arief</v>
       </c>
-      <c r="D19" s="8" t="str">
+      <c r="D19" s="6" t="str">
         <f t="shared" si="0"/>
         <v>DI</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="7">
         <v>37811</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="8" t="s">
         <v>18</v>
       </c>
       <c r="J19" s="3"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="8">
+      <c r="B20" s="6">
         <v>12</v>
       </c>
-      <c r="C20" s="6" t="str">
+      <c r="C20" s="4" t="str">
         <f>PROPER(daftar_member!B15)</f>
         <v>Indah Permata</v>
       </c>
-      <c r="D20" s="8" t="str">
+      <c r="D20" s="6" t="str">
         <f t="shared" si="0"/>
         <v>IN</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="8" t="s">
         <v>19</v>
       </c>
       <c r="J20" s="3"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="8">
+      <c r="B21" s="6">
         <v>13</v>
       </c>
-      <c r="C21" s="6" t="str">
+      <c r="C21" s="4" t="str">
         <f>PROPER(daftar_member!B16)</f>
         <v>Erwin Saputra</v>
       </c>
-      <c r="D21" s="8" t="str">
+      <c r="D21" s="6" t="str">
         <f t="shared" si="0"/>
         <v>ER</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="7">
         <v>36960</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="8" t="s">
         <v>20</v>
       </c>
       <c r="J21" s="3"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="8">
+      <c r="B22" s="6">
         <v>14</v>
       </c>
-      <c r="C22" s="6" t="str">
+      <c r="C22" s="4" t="str">
         <f>PROPER(daftar_member!B17)</f>
         <v>Rina Fauziah</v>
       </c>
-      <c r="D22" s="8" t="str">
+      <c r="D22" s="6" t="str">
         <f t="shared" si="0"/>
         <v>RI</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J22" s="3"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="8">
+      <c r="B23" s="6">
         <v>15</v>
       </c>
-      <c r="C23" s="6" t="str">
+      <c r="C23" s="4" t="str">
         <f>PROPER(daftar_member!B18)</f>
         <v>Hasan Basri</v>
       </c>
-      <c r="D23" s="8" t="str">
+      <c r="D23" s="6" t="str">
         <f t="shared" si="0"/>
         <v>HA</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="7">
         <v>37262</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="8" t="s">
         <v>22</v>
       </c>
       <c r="J23" s="3"/>
@@ -1153,82 +1153,82 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="4" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>